<commit_message>
Added dynamic data filtering, file outputs, began implentation of dept import.
NEW FEATURES:
1. You can now change the data filters during execution without having to change the code.

2. You can now export search data to a file rather than to the console. This is especially helpful for larger data searches. These export files are in a subfolder within the data folder hidden by .gitignore.

3. You can clear the console! Kind of.

4. You can test the abbreviatedClasses import method in the ClassList.java file.

TWO KNOWN BUGS:
1. The dept by college excel sheet throws a NullPointerExection when trying to read the College of Military Science, absolutely no clue why.

2. The technical course data filter is locked at false (doesn't include technical courses). Looking
</commit_message>
<xml_diff>
--- a/data/List_of_Departments.xlsx
+++ b/data/List_of_Departments.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Test\Documents\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4329DB79-CE9E-45A8-A33D-31F36DF2C4E7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6C54D904-E432-404F-98D1-8E912B88D8E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7152D3A1-8DA5-4EF1-AF8E-787FF399B030}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="29070" windowHeight="16500" xr2:uid="{7152D3A1-8DA5-4EF1-AF8E-787FF399B030}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="219">
   <si>
     <t>Academic Advising</t>
   </si>
@@ -618,9 +614,6 @@
     <t>ASTRON</t>
   </si>
   <si>
-    <t>American Sign Language</t>
-  </si>
-  <si>
     <t>ASL</t>
   </si>
   <si>
@@ -685,9 +678,6 @@
   </si>
   <si>
     <t>ACADAFF</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>School of Health and Rehabilitation Sciences</t>
@@ -1160,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2779B64-F34F-4E1B-B363-08894FBCCAFD}">
-  <dimension ref="A1:BO91"/>
+  <dimension ref="A1:BR91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E15" sqref="E15:Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1243,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>125</v>
@@ -1278,7 +1268,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>164</v>
@@ -1292,28 +1282,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>194</v>
@@ -1589,10 +1579,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>191</v>
@@ -1654,28 +1644,28 @@
         <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>184</v>
@@ -1725,7 +1715,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>193</v>
@@ -1866,7 +1856,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>72</v>
@@ -1881,7 +1871,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>181</v>
@@ -1929,7 +1919,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>186</v>
@@ -1957,10 +1947,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>193</v>

</xml_diff>